<commit_message>
Documentação completa, junto com o manual de instalação
</commit_message>
<xml_diff>
--- a/Documentação-FungiTech/dias projeto.xlsx
+++ b/Documentação-FungiTech/dias projeto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/alexandre_nichiojr_sptech_school/Documents/Área de Trabalho/temp/Sprint2/fungitech/Documentação/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/caue_oliveira_sptech_school/Documents/Documentos/fungitech/Documentação-FungiTech/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{7921C507-8602-4C65-94DE-797162BBF46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FCD348B-DAA4-44B7-BBEA-09AA7136CFBA}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{7921C507-8602-4C65-94DE-797162BBF46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D709139-F840-43AB-80E1-6FCD9B1FA386}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1A1EC1B0-117D-4488-A9B2-9140695C43A9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t>FungiTech Solutions</t>
   </si>
@@ -159,6 +159,36 @@
   </si>
   <si>
     <t xml:space="preserve">45 dias </t>
+  </si>
+  <si>
+    <t>Integração da API no tela de login e cadastro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual de Instalação </t>
+  </si>
+  <si>
+    <t>Arduino conectado no Banco de Dados</t>
+  </si>
+  <si>
+    <t>Site institucional - Versão Final</t>
+  </si>
+  <si>
+    <t>Dashboards Conectadas</t>
+  </si>
+  <si>
+    <t>Fluxogramas de processos de atendimento</t>
+  </si>
+  <si>
+    <t>Ferramenta de Help Desk</t>
+  </si>
+  <si>
+    <t>Documentação de GMUD</t>
+  </si>
+  <si>
+    <t>Modelagem do Banco de Dados - Versão Final</t>
+  </si>
+  <si>
+    <t>Distribuição dos Servidores locais em três máquinas</t>
   </si>
 </sst>
 </file>
@@ -612,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA239CA2-9EBD-432E-8F72-8EAF8073DA70}">
-  <dimension ref="D1:E27"/>
+  <dimension ref="D1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E27"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -817,16 +847,92 @@
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="3">
+        <v>45427</v>
+      </c>
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="3">
+        <v>45433</v>
+      </c>
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="3">
+        <v>45455</v>
+      </c>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="3">
+        <v>45456</v>
+      </c>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="3">
+        <v>45456</v>
+      </c>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="3">
+        <v>45432</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="3">
+        <v>45440</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" s="3">
+        <v>45438</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="3">
+        <v>45416</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="3">
+        <v>45425</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -836,20 +942,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="32844186-265b-4793-912a-671da4ac73b2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="32844186-265b-4793-912a-671da4ac73b2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1074,19 +1180,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8D3B4A7-6634-4FBA-953D-DC45436532DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{720BC78E-D489-403E-9131-3B0F5F7D2102}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="32844186-265b-4793-912a-671da4ac73b2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8D3B4A7-6634-4FBA-953D-DC45436532DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>